<commit_message>
Adding updated files for Lab 0 and added new files for Lab 1
</commit_message>
<xml_diff>
--- a/Lab 0/Marble Data (Part 2).xlsx
+++ b/Lab 0/Marble Data (Part 2).xlsx
@@ -68,7 +68,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -88,6 +88,10 @@
     <font>
       <b/>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -123,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -147,6 +151,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -923,11 +930,11 @@
       <c r="B18" s="7">
         <v>0.09953223933</v>
       </c>
-      <c r="C18" s="7">
-        <v>0.09953223933</v>
+      <c r="C18" s="8">
+        <v>0.1231485102</v>
       </c>
       <c r="D18" s="7">
-        <v>0.09953223933</v>
+        <v>0.07415449338</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>

</xml_diff>